<commit_message>
Update for ballot reconciliation
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-csc.xlsx
+++ b/build/output/StructureDefinition-pacio-csc.xlsx
@@ -1196,7 +1196,7 @@
 </t>
   </si>
   <si>
-    <t>Should point to...</t>
+    <t>Each cognitive status observation in the collection.</t>
   </si>
   <si>
     <t>This observation is a group observation (e.g. a battery, a panel of tests, a set of vital sign measurements) that includes the target as a member of the group.</t>
@@ -1218,7 +1218,7 @@
 </t>
   </si>
   <si>
-    <t>Should point back to...</t>
+    <t>Should point back to the QuestionnaireResponse that this resource is derived from.</t>
   </si>
   <si>
     <t>The target resource that represents a measurement from which this observation value is derived. For example, a calculated anion gap or a fetal measurement based on an ultrasound image.</t>

</xml_diff>